<commit_message>
ASP Industrial visit and workshop data added in excel sheet it needs formatting
</commit_message>
<xml_diff>
--- a/C2/ASP Data/Latest on 27 July/expert lecture 2016-17 to 2019-2020.xlsx
+++ b/C2/ASP Data/Latest on 27 July/expert lecture 2016-17 to 2019-2020.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="9555"/>
   </bookViews>
   <sheets>
     <sheet name="EXpert Lecture 2019-2020 " sheetId="5" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Expert Lecture 2017-2018" sheetId="7" r:id="rId3"/>
     <sheet name="2016-2017" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -420,8 +420,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -548,6 +548,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1551,9 +1558,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1563,21 +1567,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1590,37 +1579,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1635,15 +1606,54 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1653,11 +1663,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2845,17 +2852,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="23" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="81" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" style="81" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" style="85" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="23" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" style="23" customWidth="1"/>
@@ -2900,15 +2907,15 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A4" s="98" t="s">
+      <c r="A4" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="18.75" customHeight="1">
@@ -2924,14 +2931,14 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="101"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="101"/>
+      <c r="B6" s="100"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
       <c r="G6" s="97"/>
       <c r="H6" s="5"/>
     </row>
@@ -3088,11 +3095,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -3110,53 +3117,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
       <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:9" ht="18.75">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
       <c r="H2" s="37"/>
       <c r="I2" s="37"/>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
       <c r="H3" s="38"/>
       <c r="I3" s="38"/>
     </row>
     <row r="4" spans="1:9" ht="18.75">
-      <c r="A4" s="107" t="s">
+      <c r="A4" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="107"/>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
       <c r="H4" s="39"/>
       <c r="I4" s="39"/>
     </row>
@@ -3270,75 +3277,75 @@
       <c r="H10" s="59"/>
     </row>
     <row r="11" spans="1:9" ht="45" customHeight="1">
-      <c r="A11" s="103">
+      <c r="A11" s="106">
         <v>3</v>
       </c>
-      <c r="B11" s="104" t="s">
+      <c r="B11" s="107" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="105" t="s">
+      <c r="C11" s="108" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="104" t="s">
+      <c r="D11" s="107" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="74">
         <v>43344</v>
       </c>
-      <c r="F11" s="104" t="s">
+      <c r="F11" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="102" t="s">
+      <c r="G11" s="105" t="s">
         <v>46</v>
       </c>
       <c r="H11" s="59"/>
     </row>
     <row r="12" spans="1:9" ht="34.5" customHeight="1">
-      <c r="A12" s="103"/>
-      <c r="B12" s="104"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="104"/>
+      <c r="A12" s="106"/>
+      <c r="B12" s="107"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="107"/>
       <c r="E12" s="74">
         <v>43345</v>
       </c>
-      <c r="F12" s="104"/>
-      <c r="G12" s="102"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="105"/>
       <c r="H12" s="59"/>
     </row>
     <row r="13" spans="1:9" ht="19.5" customHeight="1">
-      <c r="A13" s="103">
+      <c r="A13" s="106">
         <v>4</v>
       </c>
-      <c r="B13" s="104" t="s">
+      <c r="B13" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="105" t="s">
+      <c r="C13" s="108" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="104" t="s">
+      <c r="D13" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="106">
+      <c r="E13" s="109">
         <v>43473</v>
       </c>
       <c r="F13" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="102" t="s">
+      <c r="G13" s="105" t="s">
         <v>73</v>
       </c>
       <c r="H13" s="59"/>
     </row>
     <row r="14" spans="1:9" ht="31.5" customHeight="1">
-      <c r="A14" s="103"/>
-      <c r="B14" s="104"/>
-      <c r="C14" s="105"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="105"/>
+      <c r="A14" s="106"/>
+      <c r="B14" s="107"/>
+      <c r="C14" s="108"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="108"/>
       <c r="F14" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="102"/>
+      <c r="G14" s="105"/>
       <c r="H14" s="59"/>
     </row>
     <row r="15" spans="1:9" ht="72" customHeight="1" thickBot="1">
@@ -3386,22 +3393,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="G11:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="72" orientation="portrait"/>
@@ -3412,11 +3419,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C9" sqref="C9:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3433,49 +3440,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
       <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="18.75">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8" ht="15.75">
-      <c r="A3" s="124" t="s">
+      <c r="A3" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8" ht="18.75">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="113" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="125"/>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
-      <c r="E4" s="125"/>
-      <c r="F4" s="125"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
     </row>
@@ -3527,90 +3534,90 @@
       <c r="G8" s="33"/>
     </row>
     <row r="9" spans="1:8" ht="15.75">
-      <c r="A9" s="111">
+      <c r="A9" s="114">
         <v>1</v>
       </c>
-      <c r="B9" s="113" t="s">
+      <c r="B9" s="116" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="115" t="s">
+      <c r="C9" s="118" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="115" t="s">
+      <c r="D9" s="118" t="s">
         <v>94</v>
       </c>
       <c r="E9" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="118" t="s">
+      <c r="F9" s="120" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75">
-      <c r="A10" s="112"/>
-      <c r="B10" s="114"/>
-      <c r="C10" s="116"/>
-      <c r="D10" s="114"/>
+      <c r="A10" s="115"/>
+      <c r="B10" s="117"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="117"/>
       <c r="E10" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="119"/>
+      <c r="F10" s="121"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="120">
+      <c r="A11" s="122">
         <v>2</v>
       </c>
-      <c r="B11" s="117" t="s">
+      <c r="B11" s="123" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="117" t="s">
+      <c r="C11" s="123" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="117" t="s">
+      <c r="D11" s="123" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="117" t="s">
+      <c r="E11" s="123" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="121" t="s">
+      <c r="F11" s="124" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A12" s="112"/>
-      <c r="B12" s="114"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="119"/>
+      <c r="A12" s="115"/>
+      <c r="B12" s="117"/>
+      <c r="C12" s="117"/>
+      <c r="D12" s="117"/>
+      <c r="E12" s="117"/>
+      <c r="F12" s="121"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="111">
+      <c r="A13" s="114">
         <v>3</v>
       </c>
-      <c r="B13" s="113" t="s">
+      <c r="B13" s="116" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="115" t="s">
+      <c r="C13" s="118" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="117" t="s">
+      <c r="D13" s="123" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="117" t="s">
+      <c r="E13" s="123" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="118" t="s">
+      <c r="F13" s="120" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="112"/>
-      <c r="B14" s="114"/>
-      <c r="C14" s="116"/>
-      <c r="D14" s="114"/>
-      <c r="E14" s="114"/>
-      <c r="F14" s="119"/>
+      <c r="A14" s="115"/>
+      <c r="B14" s="117"/>
+      <c r="C14" s="119"/>
+      <c r="D14" s="117"/>
+      <c r="E14" s="117"/>
+      <c r="F14" s="121"/>
     </row>
     <row r="15" spans="1:8" ht="63.75" thickBot="1">
       <c r="A15" s="34">
@@ -3644,15 +3651,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="F9:F10"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
@@ -3665,16 +3663,25 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -3692,49 +3699,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
       <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="107" t="s">
+      <c r="A4" s="101" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="107"/>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
     </row>
@@ -3793,10 +3800,10 @@
       <c r="G8" s="33"/>
     </row>
     <row r="9" spans="1:8" ht="36" customHeight="1">
-      <c r="A9" s="126">
+      <c r="A9" s="125">
         <v>1</v>
       </c>
-      <c r="B9" s="128" t="s">
+      <c r="B9" s="127" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="46" t="s">
@@ -3808,13 +3815,13 @@
       <c r="E9" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="128" t="s">
+      <c r="F9" s="127" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="48.75" customHeight="1" thickBot="1">
-      <c r="A10" s="132"/>
-      <c r="B10" s="133"/>
+      <c r="A10" s="126"/>
+      <c r="B10" s="128"/>
       <c r="C10" s="53" t="s">
         <v>47</v>
       </c>
@@ -3824,16 +3831,16 @@
       <c r="E10" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="133"/>
+      <c r="F10" s="128"/>
     </row>
     <row r="11" spans="1:8" ht="35.25" customHeight="1">
-      <c r="A11" s="126">
+      <c r="A11" s="125">
         <v>2</v>
       </c>
-      <c r="B11" s="128" t="s">
+      <c r="B11" s="127" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="130" t="s">
+      <c r="C11" s="131" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="49" t="s">
@@ -3842,51 +3849,51 @@
       <c r="E11" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="128" t="s">
+      <c r="F11" s="127" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A12" s="127"/>
-      <c r="B12" s="129"/>
-      <c r="C12" s="131"/>
+      <c r="A12" s="129"/>
+      <c r="B12" s="130"/>
+      <c r="C12" s="132"/>
       <c r="D12" s="45" t="s">
         <v>53</v>
       </c>
       <c r="E12" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="129"/>
+      <c r="F12" s="130"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1">
-      <c r="A13" s="126">
+      <c r="A13" s="125">
         <v>3</v>
       </c>
-      <c r="B13" s="128" t="s">
+      <c r="B13" s="127" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="130" t="s">
+      <c r="C13" s="131" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="128" t="s">
+      <c r="D13" s="127" t="s">
         <v>56</v>
       </c>
       <c r="E13" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="128" t="s">
+      <c r="F13" s="127" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" customHeight="1" thickBot="1">
-      <c r="A14" s="127"/>
-      <c r="B14" s="129"/>
-      <c r="C14" s="131"/>
-      <c r="D14" s="129"/>
+      <c r="A14" s="129"/>
+      <c r="B14" s="130"/>
+      <c r="C14" s="132"/>
+      <c r="D14" s="130"/>
       <c r="E14" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="129"/>
+      <c r="F14" s="130"/>
     </row>
     <row r="15" spans="1:8" ht="58.5" customHeight="1" thickBot="1">
       <c r="A15" s="56">
@@ -3978,13 +3985,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="F9:F10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
@@ -3994,6 +3994,13 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="76" orientation="portrait" r:id="rId1"/>

</xml_diff>